<commit_message>
adding variant effects table to excel files andd adding dlx6 gene
</commit_message>
<xml_diff>
--- a/ccdc66_excel.xlsx
+++ b/ccdc66_excel.xlsx
@@ -10,13 +10,14 @@
     <sheet name="ccdc66_to_excel" sheetId="1" r:id="rId1"/>
     <sheet name="vcf color" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="variant effect" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="208">
   <si>
     <t>chr20</t>
   </si>
@@ -613,6 +614,33 @@
   </si>
   <si>
     <t>chloe</t>
+  </si>
+  <si>
+    <t>20_33747568_C/A</t>
+  </si>
+  <si>
+    <t>20:33747568</t>
+  </si>
+  <si>
+    <t>NM_001168012.1</t>
+  </si>
+  <si>
+    <t>Transcript</t>
+  </si>
+  <si>
+    <t>stop_gained</t>
+  </si>
+  <si>
+    <t>G/*</t>
+  </si>
+  <si>
+    <t>Gga/Tga</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>IMPACT=HIGH;STRAND=-1</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1155,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1137,6 +1165,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5046,4 +5075,63 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7">
+        <v>476582</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="7">
+        <v>404</v>
+      </c>
+      <c r="I1" s="7">
+        <v>94</v>
+      </c>
+      <c r="J1" s="7">
+        <v>32</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>